<commit_message>
Actividad 1. Reunión de revisión inicial
</commit_message>
<xml_diff>
--- a/src/Materias primas.xlsx
+++ b/src/Materias primas.xlsx
@@ -75,7 +75,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,6 +88,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -171,10 +181,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -184,8 +195,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Moneda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -510,7 +523,7 @@
       <c r="D2" s="2">
         <v>1000</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="5">
         <v>1</v>
       </c>
       <c r="F2" s="2" t="s">
@@ -530,7 +543,7 @@
       <c r="D3" s="2">
         <v>1000</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="5">
         <v>1</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -550,7 +563,7 @@
       <c r="D4" s="2">
         <v>1000</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="5">
         <v>1</v>
       </c>
       <c r="F4" s="2" t="s">

</xml_diff>